<commit_message>
Turn off status hadir in ori implementation
</commit_message>
<xml_diff>
--- a/public/template/input_pelaksanaan_ori.xlsx
+++ b/public/template/input_pelaksanaan_ori.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\eoribr\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3C2CDA-3507-4B59-9FDE-25A0B2BC91AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD847BC-17C2-435B-B876-A795A10A5A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B0BF7AAE-24AC-4F0D-968C-5C193EC9E427}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>kelurahan</t>
   </si>
@@ -60,9 +60,6 @@
     <t>no_hp</t>
   </si>
   <si>
-    <t>status_kehadiran</t>
-  </si>
-  <si>
     <t>tgl_lahir</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>+62-60-487-6441</t>
   </si>
   <si>
-    <t>Hadir</t>
-  </si>
-  <si>
     <t>Tgk. Endra Sinaga, M.Ak</t>
   </si>
   <si>
@@ -124,9 +118,6 @@
   </si>
   <si>
     <t>+62 (68) 767-2411</t>
-  </si>
-  <si>
-    <t>Tidak Hadir</t>
   </si>
   <si>
     <t>Warsa Sihombing</t>
@@ -545,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC06F78-18F4-46E8-A2F3-6073E93FA2B2}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="L1" sqref="L1:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +557,7 @@
     <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +565,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -595,241 +586,220 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
       </c>
       <c r="C2" s="1">
         <v>44015</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>5165231857345387</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2">
         <v>2421294302221874</v>
       </c>
       <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K2">
         <v>12345678</v>
       </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>1787627949720519</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>1241708200112771</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K3">
         <v>12345678</v>
       </c>
-      <c r="L3" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4">
         <v>8274059656814802</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G4">
         <v>9069876114534172</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K4">
         <v>12345678</v>
       </c>
-      <c r="L4" t="s">
-        <v>26</v>
-      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <v>3941971284224411</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G5">
         <v>9721560736052100</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K5">
         <v>12345678</v>
       </c>
-      <c r="L5" t="s">
-        <v>26</v>
-      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E6">
         <v>5265716823376987</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G6">
         <v>6806205674938460</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K6">
         <v>12345678</v>
       </c>
-      <c r="L6" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
       </c>
       <c r="E7">
         <v>2576882185629032</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G7">
         <v>3460517811766894</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K7">
         <v>12345678</v>
-      </c>
-      <c r="L7" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>